<commit_message>
Insert W2 into f1040-2018
</commit_message>
<xml_diff>
--- a/Federal/f1040-2018.xlsx
+++ b/Federal/f1040-2018.xlsx
@@ -9,7 +9,33 @@
   </bookViews>
   <sheets>
     <sheet name="IRS f1040" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="W2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="false" name="Line1" vbProcedure="false">W2!$D$6</definedName>
+    <definedName function="false" hidden="false" name="Line10" vbProcedure="false">W2!$D$15</definedName>
+    <definedName function="false" hidden="false" name="Line11" vbProcedure="false">W2!$D$16</definedName>
+    <definedName function="false" hidden="false" name="Line12a" vbProcedure="false">W2!$E$17</definedName>
+    <definedName function="false" hidden="false" name="Line12b" vbProcedure="false">W2!$E$18</definedName>
+    <definedName function="false" hidden="false" name="Line12c" vbProcedure="false">W2!$E$19</definedName>
+    <definedName function="false" hidden="false" name="Line12d" vbProcedure="false">W2!$E$20</definedName>
+    <definedName function="false" hidden="false" name="Line13" vbProcedure="false">W2!$D$21</definedName>
+    <definedName function="false" hidden="false" name="Line14" vbProcedure="false">W2!$D$22</definedName>
+    <definedName function="false" hidden="false" name="Line15" vbProcedure="false">W2!$E$23</definedName>
+    <definedName function="false" hidden="false" name="Line16" vbProcedure="false">W2!$D$24</definedName>
+    <definedName function="false" hidden="false" name="Line17" vbProcedure="false">W2!$D$25</definedName>
+    <definedName function="false" hidden="false" name="Line18" vbProcedure="false">W2!$D$26</definedName>
+    <definedName function="false" hidden="false" name="Line19" vbProcedure="false">W2!$D$27</definedName>
+    <definedName function="false" hidden="false" name="Line2" vbProcedure="false">W2!$D$7</definedName>
+    <definedName function="false" hidden="false" name="Line20" vbProcedure="false">W2!$D$28</definedName>
+    <definedName function="false" hidden="false" name="Line3" vbProcedure="false">W2!$D$8</definedName>
+    <definedName function="false" hidden="false" name="Line4" vbProcedure="false">W2!$D$9</definedName>
+    <definedName function="false" hidden="false" name="Line5" vbProcedure="false">W2!$D$10</definedName>
+    <definedName function="false" hidden="false" name="Line6" vbProcedure="false">W2!$D$11</definedName>
+    <definedName function="false" hidden="false" name="Line7" vbProcedure="false">W2!$D$12</definedName>
+    <definedName function="false" hidden="false" name="Line8" vbProcedure="false">W2!$D$13</definedName>
+    <definedName function="false" hidden="false" name="Line9" vbProcedure="false">W2!$D$14</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="114">
   <si>
     <t xml:space="preserve">Form  1040 (2018)        Department of the Treasury--Internal Revenue Service       Page 2</t>
   </si>
@@ -269,6 +295,132 @@
   <si>
     <t xml:space="preserve">Estimated tax penalty (see instructions)</t>
   </si>
+  <si>
+    <t xml:space="preserve">2016 Form W-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employer Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wages, tips, other compensation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federal income tax withheld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social security wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social security tax withheld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicare wages and tips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medicare tax withheld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social security tips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allocated tips</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dependent care benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nonqualified plans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12a.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12b.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12c.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12d.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State wages, tips, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State income tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local wages, tips, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local income tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locality name</t>
+  </si>
 </sst>
 </file>
 
@@ -278,7 +430,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -323,8 +475,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -334,7 +492,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBCE4E5"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFE6E6E6"/>
       </patternFill>
     </fill>
     <fill>
@@ -343,8 +501,14 @@
         <bgColor rgb="FF808080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E6E6"/>
+        <bgColor rgb="FFBCE4E5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -401,6 +565,34 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -432,7 +624,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -449,23 +641,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -522,6 +714,54 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,7 +780,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFE6E6E6"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -607,8 +847,8 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,7 +883,10 @@
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="n">
+        <f aca="false">W2!D6</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -655,9 +898,9 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -671,7 +914,7 @@
       <c r="E4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -683,9 +926,9 @@
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="7"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -699,7 +942,7 @@
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -711,9 +954,9 @@
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="7"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -727,7 +970,7 @@
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -739,9 +982,9 @@
       <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="7"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
@@ -755,7 +998,7 @@
       <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
@@ -763,9 +1006,9 @@
         <v>18</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="7"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
@@ -779,7 +1022,7 @@
       <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="4" t="n">
         <f aca="false">SUM(F2:F11)+D11</f>
         <v>0</v>
       </c>
@@ -790,9 +1033,9 @@
         <v>21</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -806,7 +1049,7 @@
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="4" t="n">
         <f aca="false">F12-D13</f>
         <v>0</v>
       </c>
@@ -873,7 +1116,7 @@
       <c r="E20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="8"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
@@ -887,7 +1130,7 @@
       <c r="E21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
@@ -901,7 +1144,7 @@
       <c r="E22" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="8" t="n">
+      <c r="F22" s="4" t="n">
         <f aca="false">F14-F20-F21</f>
         <v>0</v>
       </c>
@@ -914,9 +1157,9 @@
         <v>35</v>
       </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="8"/>
+      <c r="D23" s="4"/>
       <c r="E23" s="12"/>
-      <c r="F23" s="7"/>
+      <c r="F23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="13"/>
@@ -924,11 +1167,11 @@
         <v>36</v>
       </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="8"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="14" t="n">
         <v>11</v>
       </c>
-      <c r="F24" s="8" t="n">
+      <c r="F24" s="4" t="n">
         <f aca="false">D23+D24</f>
         <v>0</v>
       </c>
@@ -941,9 +1184,9 @@
         <v>38</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="8"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="13"/>
@@ -951,11 +1194,11 @@
         <v>39</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="8"/>
+      <c r="D26" s="4"/>
       <c r="E26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="8" t="n">
+      <c r="F26" s="4" t="n">
         <f aca="false">D25+D26</f>
         <v>0</v>
       </c>
@@ -972,7 +1215,7 @@
       <c r="E27" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F27" s="8" t="n">
+      <c r="F27" s="4" t="n">
         <f aca="false">MAX(F24-F26,0)</f>
         <v>0</v>
       </c>
@@ -989,7 +1232,7 @@
       <c r="E28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
@@ -1020,7 +1263,10 @@
       <c r="E30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="8"/>
+      <c r="F30" s="4" t="n">
+        <f aca="false">W2!D7</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18" t="s">
@@ -1042,9 +1288,9 @@
       <c r="C32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -1056,9 +1302,9 @@
       <c r="C33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="7"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
@@ -1070,9 +1316,9 @@
       <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
@@ -1084,9 +1330,9 @@
       <c r="C35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="7"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
@@ -1100,7 +1346,7 @@
       <c r="E36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F36" s="8" t="n">
+      <c r="F36" s="4" t="n">
         <f aca="false">SUM(D32:D35)</f>
         <v>0</v>
       </c>
@@ -1117,7 +1363,7 @@
       <c r="E37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="8" t="n">
+      <c r="F37" s="4" t="n">
         <f aca="false">F30+F36</f>
         <v>0</v>
       </c>
@@ -1176,12 +1422,12 @@
       <c r="C41" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="8" t="n">
+      <c r="D41" s="4" t="n">
         <f aca="false">F39-F40</f>
         <v>0</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
@@ -1242,4 +1488,377 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="4.8"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="28" t="str">
+        <f aca="false">"13."</f>
+        <v>13.</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="2" t="str">
+        <f aca="false">"13."</f>
+        <v>13.</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="22"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>